<commit_message>
progress on scraping postal codes
</commit_message>
<xml_diff>
--- a/scraped-data.xlsx
+++ b/scraped-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leocr\Desktop\lbc-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{287E2657-A79E-4EDA-8E38-FECBB60B5408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AED3BD0B-84FC-4BA6-AC9D-76C411D39F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13665" yWindow="45" windowWidth="10335" windowHeight="12855" xr2:uid="{AAE6B178-521F-4F95-86C2-F3FCE3B5AC85}"/>
+    <workbookView xWindow="13665" yWindow="45" windowWidth="10335" windowHeight="12855" xr2:uid="{A28B734C-04CC-48EB-BC74-C851A2033DD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
-  <si>
-    <t>location</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+  <si>
+    <t>number</t>
   </si>
   <si>
     <t>url</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>33400 Talence</t>
-  </si>
-  <si>
-    <t>https://leboncoin.fr</t>
-  </si>
-  <si>
-    <t>14000 Caen</t>
-  </si>
-  <si>
-    <t>75000 Paris</t>
+    <t>title</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>siret</t>
+  </si>
+  <si>
+    <t>09 72 45 60 82</t>
+  </si>
+  <si>
+    <t>https://www.leboncoin.fr/ventes_immobilieres/2132576632.htm</t>
+  </si>
+  <si>
+    <t>Maison 6 pièces 210 m²_x000D_
+6 Pièces · _x000D_
+210 m² · _x000D_
+Bourg-en-Bresse 01000 _x000D_
+460 000 €_x000D_
+2 190 €/m²_x000D_
+01/12/2022 à 15:18</t>
+  </si>
+  <si>
+    <t>THIBAUD VENET IMMOBIL</t>
+  </si>
+  <si>
+    <t>09 86 87 17 08</t>
+  </si>
+  <si>
+    <t>https://www.leboncoin.fr/ventes_immobilieres/2245750085.htm</t>
+  </si>
+  <si>
+    <t>Maison 10 pièces 670 m²_x000D_
+10 Pièces · _x000D_
+670 m² · _x000D_
+Bourg-en-Bresse 01000 _x000D_
+365 000 €_x000D_
+545 €/m²_x000D_
+01/12/2022 à 15:04</t>
+  </si>
+  <si>
+    <t>LAZARE INVEST IMMO</t>
+  </si>
+  <si>
+    <t>https://www.leboncoin.fr/ventes_immobilieres/2235912836.htm</t>
+  </si>
+  <si>
+    <t>Maison 4 pièces 166 m²_x000D_
+4 Pièces · _x000D_
+166 m² · _x000D_
+Val-Revermont 01370 _x000D_
+289 000 €_x000D_
+1 741 €/m²_x000D_
+01/12/2022 à 13:14</t>
   </si>
 </sst>
 </file>
@@ -92,8 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,14 +452,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FDFAF9-5401-4115-976F-DA24939B9D3E}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A80618-5BC9-4C59-8E69-1A3434695DF6}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,38 +469,62 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>612457896</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>88188484500010</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>82061894000028</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>88188484500010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>